<commit_message>
Fixed booleans on the sheet and added prefixes for tags and genres
</commit_message>
<xml_diff>
--- a/protege/sheet.xlsx
+++ b/protege/sheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="games" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Counter-Strike: Global Offensive (CS: GO) expands upon the team-based action gameplay that it pioneered when it was launched 19 years ago. CS: GO features new maps, characters, weapons, and game modes, and delivers updated versions of the classic CS content (de_dust2, etc.).</t>
   </si>
   <si>
-    <t xml:space="preserve">False</t>
+    <t xml:space="preserve">false</t>
   </si>
   <si>
     <t xml:space="preserve">21-08-2012</t>
@@ -635,7 +635,7 @@
     <t xml:space="preserve">10-12-2015</t>
   </si>
   <si>
-    <t xml:space="preserve">True</t>
+    <t xml:space="preserve">true</t>
   </si>
   <si>
     <t xml:space="preserve">very nice game ~!</t>
@@ -963,6 +963,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">玲音</t>
     </r>
@@ -1345,9 +1346,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1375,6 +1377,7 @@
       <sz val="10"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1419,7 +1422,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1432,18 +1435,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -1455,26 +1462,27 @@
   </sheetPr>
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="235.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="240.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1539,7 @@
       <c r="I2" s="0" t="n">
         <v>39.99</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="0" t="s">
@@ -1863,10 +1871,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.76"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3619,10 +3628,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3759,10 +3769,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4043,10 +4054,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.02"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4788,13 +4800,14 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4939,10 +4952,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4995,23 +5009,25 @@
   </sheetPr>
   <dimension ref="B1:L55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="2.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="182.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6022,7 +6038,7 @@
       <c r="K29" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="L29" s="4" t="s">
         <v>268</v>
       </c>
     </row>

</xml_diff>